<commit_message>
added colors to the animal names
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -17,6 +17,7 @@
     <r>
       <rPr>
         <b val="true"/>
+        <color indexed="54"/>
         <sz val="11.0"/>
         <rFont val="Calibri"/>
       </rPr>
@@ -27,6 +28,7 @@
     <r>
       <rPr>
         <b val="true"/>
+        <color indexed="54"/>
         <sz val="11.0"/>
         <rFont val="Calibri"/>
       </rPr>
@@ -34,25 +36,67 @@
     </r>
   </si>
   <si>
-    <t>Zebra</t>
+    <r>
+      <rPr>
+        <color indexed="50"/>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Zebra</t>
+    </r>
   </si>
   <si>
     <t>Trecias</t>
   </si>
   <si>
-    <t>Giraffe</t>
-  </si>
-  <si>
-    <t>Wolf</t>
-  </si>
-  <si>
-    <t>Lion</t>
-  </si>
-  <si>
-    <t>Otter</t>
-  </si>
-  <si>
-    <t>Sea Lion</t>
+    <r>
+      <rPr>
+        <color indexed="8"/>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Giraffe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color indexed="12"/>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Wolf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color indexed="10"/>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Lion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color indexed="53"/>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Otter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color indexed="57"/>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Sea Lion</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -60,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -72,6 +116,37 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <b val="true"/>
+      <color indexed="54"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="50"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="57"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>